<commit_message>
ppt and project changes - added skeleton to ppt
</commit_message>
<xml_diff>
--- a/project.xlsx
+++ b/project.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dschlesinger\code\ongoing\openaiworkshop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E8CF5F2-987F-4DDF-AC40-C0AF9BB5BE40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF91FE9B-88AF-497C-9740-A1F348BC68D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-3480" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="project" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">project!$A$1:$D$14</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">project!$A$1:$D$16</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="26">
   <si>
     <t>Tasks</t>
   </si>
@@ -108,6 +108,12 @@
   </si>
   <si>
     <t>10- Bonus - Search your company's URLs with OpenAI</t>
+  </si>
+  <si>
+    <t>Create ppt skeleton</t>
+  </si>
+  <si>
+    <t>turn all Denise's labs into notebooks</t>
   </si>
 </sst>
 </file>
@@ -978,10 +984,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1005,7 +1011,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1047,7 +1053,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -1061,7 +1067,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -1083,7 +1089,7 @@
         <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="D7" t="s">
         <v>12</v>
@@ -1103,7 +1109,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -1131,7 +1137,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -1173,7 +1179,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -1187,11 +1193,44 @@
         <v>12</v>
       </c>
     </row>
+    <row r="15" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:D14" xr:uid="{00000000-0009-0000-0000-000000000000}">
+  <autoFilter ref="A1:D16" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <filterColumn colId="2">
       <filters>
-        <filter val="Vladi"/>
+        <filter val="Denise"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="3">
+      <filters>
+        <filter val="tbd"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>